<commit_message>
Add productBaclog from isoftware
</commit_message>
<xml_diff>
--- a/03-Documentation/Team3_Product Backlog-Matrix_frame_work_HU V2.0.xlsx
+++ b/03-Documentation/Team3_Product Backlog-Matrix_frame_work_HU V2.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Desktop\Sexto Semestre\Aplicaciones Web 8516 Jueves 5-7\Primer Parcial\GIT\DevSolutionsT3\03-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925C894F-CC9E-4B45-A2BE-66BD1C36DC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECC19AF-1B5C-4075-AFCB-38372D4248FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog- HU" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="201">
   <si>
     <t>ITEM</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Product Backlog - Matrix frame of work HU</t>
   </si>
   <si>
-    <t>List Inventory</t>
-  </si>
-  <si>
     <t>Allow to delete products</t>
   </si>
   <si>
@@ -504,6 +501,144 @@
   </si>
   <si>
     <t>Delete invoice to the system</t>
+  </si>
+  <si>
+    <t>List Products</t>
+  </si>
+  <si>
+    <t>REQ17</t>
+  </si>
+  <si>
+    <t>REQ18</t>
+  </si>
+  <si>
+    <t>REQ19</t>
+  </si>
+  <si>
+    <t>REQ20</t>
+  </si>
+  <si>
+    <t>Add Distributor</t>
+  </si>
+  <si>
+    <t>List Distributor</t>
+  </si>
+  <si>
+    <t>Update Distributor</t>
+  </si>
+  <si>
+    <t>Delete Distributor</t>
+  </si>
+  <si>
+    <t>Registration of new Distributor</t>
+  </si>
+  <si>
+    <t>Review the list of Distributor</t>
+  </si>
+  <si>
+    <t>Allow to update the Distributor information</t>
+  </si>
+  <si>
+    <t>Remove an Distributor from the databes</t>
+  </si>
+  <si>
+    <t>Enter the order information to add a new Distributor in the database.</t>
+  </si>
+  <si>
+    <t>Enter the order list module and the system shows up a list of Distributor saved in the database</t>
+  </si>
+  <si>
+    <t>An Invoice is edited, the information about the Distributor it's modified and saved in the database.</t>
+  </si>
+  <si>
+    <t>An Invoice it's selected, searched by the Distributor id and deleated from the database</t>
+  </si>
+  <si>
+    <t>The interface shows the added Distributor</t>
+  </si>
+  <si>
+    <t>The interface shows the screen to add Distributor</t>
+  </si>
+  <si>
+    <t>The interface shows the screen to update Distributor</t>
+  </si>
+  <si>
+    <t>The interface remove the Distributor</t>
+  </si>
+  <si>
+    <t>Add Distributor  to the system</t>
+  </si>
+  <si>
+    <t>List Distributor to the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Distributor to the system </t>
+  </si>
+  <si>
+    <t>Delete Distributor to the system</t>
+  </si>
+  <si>
+    <t>Search for a Distributor</t>
+  </si>
+  <si>
+    <t>Search for a User</t>
+  </si>
+  <si>
+    <t>Search for a Product</t>
+  </si>
+  <si>
+    <t>Search for a Order</t>
+  </si>
+  <si>
+    <t>Search for a Invoice</t>
+  </si>
+  <si>
+    <t>Search Product</t>
+  </si>
+  <si>
+    <t>Search User</t>
+  </si>
+  <si>
+    <t>Search Order</t>
+  </si>
+  <si>
+    <t>Search Invoice</t>
+  </si>
+  <si>
+    <t>Search an Invoice from the databes</t>
+  </si>
+  <si>
+    <t>Search an User from the databes</t>
+  </si>
+  <si>
+    <t>Search an Order from the databes</t>
+  </si>
+  <si>
+    <t>Search Distributoruct</t>
+  </si>
+  <si>
+    <t>Search an Distributoruct from the databes</t>
+  </si>
+  <si>
+    <t>Search an Product from the databes</t>
+  </si>
+  <si>
+    <t>An Invoice it's selected, searched by the Product</t>
+  </si>
+  <si>
+    <t>An Invoice it's selected, searched by the User</t>
+  </si>
+  <si>
+    <t>An Invoice it's selected, searched by the Order</t>
+  </si>
+  <si>
+    <t>An Invoice it's selected, searched by the Invoice</t>
+  </si>
+  <si>
+    <t>An Invoice it's selected, searched by the ProdDistributoructuct</t>
+  </si>
+  <si>
+    <t>The interface shows the added Orders</t>
   </si>
 </sst>
 </file>
@@ -513,7 +648,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,11 +685,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
     </font>
     <font>
       <sz val="11"/>
@@ -623,6 +753,20 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1027,9 +1171,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,34 +1187,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1079,7 +1218,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1088,54 +1227,89 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1163,7 +1337,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1171,78 +1383,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1559,8 +1720,8 @@
   </sheetPr>
   <dimension ref="B1:Q999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1595,22 +1756,22 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G4" s="4"/>
@@ -1621,931 +1782,1297 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="M5" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="35" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="28">
+        <v>3</v>
+      </c>
+      <c r="J6" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="30" t="s">
+      <c r="C7" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="28">
+        <v>3</v>
+      </c>
+      <c r="J7" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="C8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="28">
+        <v>3</v>
+      </c>
+      <c r="J8" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="28">
+        <v>3</v>
+      </c>
+      <c r="J9" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="57" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="28">
+        <v>3</v>
+      </c>
+      <c r="J10" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="28">
+        <v>3</v>
+      </c>
+      <c r="J11" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="N11" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="28">
+        <v>3</v>
+      </c>
+      <c r="J12" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="N12" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="28">
+        <v>3</v>
+      </c>
+      <c r="J13" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I14" s="41">
         <v>3</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J14" s="42">
         <v>44902</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K14" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L14" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="30" t="s">
+      <c r="M14" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="N14" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="O14" s="44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="57" x14ac:dyDescent="0.2">
+      <c r="B15" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="31" t="s">
+      <c r="G15" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I15" s="41">
         <v>3</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J15" s="42">
         <v>44902</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="K15" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="34" t="s">
+      <c r="L15" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="M15" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="N15" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="41">
+        <v>3</v>
+      </c>
+      <c r="J16" s="42">
+        <v>44902</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N16" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="O16" s="44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="41">
+        <v>3</v>
+      </c>
+      <c r="J17" s="42">
+        <v>44902</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="N17" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="O17" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="28">
+        <v>3</v>
+      </c>
+      <c r="J18" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="N18" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="57" x14ac:dyDescent="0.2">
+      <c r="B19" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="28">
+        <v>3</v>
+      </c>
+      <c r="J19" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="N19" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="O19" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="28">
+        <v>3</v>
+      </c>
+      <c r="J20" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="N20" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="O20" s="44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="28">
+        <v>3</v>
+      </c>
+      <c r="J21" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="N21" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="O21" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="28">
+        <v>3</v>
+      </c>
+      <c r="J22" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="N22" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="O22" s="44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="H23" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="28">
+        <v>3</v>
+      </c>
+      <c r="J23" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L23" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="N23" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="O23" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="28">
+        <v>3</v>
+      </c>
+      <c r="J24" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="N24" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="O24" s="44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="H25" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="28">
+        <v>3</v>
+      </c>
+      <c r="J25" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="N25" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="O25" s="44" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="28">
+        <v>3</v>
+      </c>
+      <c r="J26" s="29">
+        <v>44902</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L26" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="36" t="s">
+      <c r="N26" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="31" t="s">
+      <c r="O26" s="41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="H27" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="30" t="s">
+      <c r="I27" s="28">
+        <v>3</v>
+      </c>
+      <c r="J27" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="N27" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O27" s="41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="31" t="s">
+      <c r="G28" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I28" s="28">
         <v>3</v>
       </c>
-      <c r="J8" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K8" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="34" t="s">
+      <c r="J28" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L28" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="N8" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="O8" s="35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="B9" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="M28" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O28" s="41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="F29" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="31">
+      <c r="G29" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="28">
         <v>3</v>
       </c>
-      <c r="J9" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K9" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="34" t="s">
+      <c r="J29" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="O9" s="35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="B10" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="30" t="s">
+      <c r="M29" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="N29" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O29" s="41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="F30" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="31">
+      <c r="G30" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="H30" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="28">
         <v>3</v>
       </c>
-      <c r="J10" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K10" s="31" t="s">
+      <c r="J30" s="29">
+        <v>44956</v>
+      </c>
+      <c r="K30" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="34" t="s">
+      <c r="L30" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="31">
-        <v>3</v>
-      </c>
-      <c r="J11" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K11" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="N11" s="36" t="s">
+      <c r="M30" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="N30" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="O11" s="35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="31">
-        <v>3</v>
-      </c>
-      <c r="J12" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="N12" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="O12" s="35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="31">
-        <v>3</v>
-      </c>
-      <c r="J13" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K13" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L13" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="N13" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="O13" s="35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="85" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="84" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="85">
-        <v>3</v>
-      </c>
-      <c r="J14" s="86">
-        <v>44902</v>
-      </c>
-      <c r="K14" s="85" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="90" t="s">
-        <v>108</v>
-      </c>
-      <c r="N14" s="89" t="s">
-        <v>109</v>
-      </c>
-      <c r="O14" s="88" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="84" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="H15" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="I15" s="85">
-        <v>3</v>
-      </c>
-      <c r="J15" s="86">
-        <v>44902</v>
-      </c>
-      <c r="K15" s="85" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="89" t="s">
-        <v>115</v>
-      </c>
-      <c r="N15" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="O15" s="88" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="85" t="s">
-        <v>134</v>
-      </c>
-      <c r="E16" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="91" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="85">
-        <v>3</v>
-      </c>
-      <c r="J16" s="86">
-        <v>44902</v>
-      </c>
-      <c r="K16" s="85" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="M16" s="89" t="s">
-        <v>121</v>
-      </c>
-      <c r="N16" s="89" t="s">
-        <v>122</v>
-      </c>
-      <c r="O16" s="88" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="85" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="85" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="85" t="s">
-        <v>125</v>
-      </c>
-      <c r="F17" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="91" t="s">
-        <v>126</v>
-      </c>
-      <c r="H17" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="I17" s="85">
-        <v>3</v>
-      </c>
-      <c r="J17" s="86">
-        <v>44902</v>
-      </c>
-      <c r="K17" s="85" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="89" t="s">
-        <v>127</v>
-      </c>
-      <c r="N17" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="O17" s="88" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="85" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="84" t="s">
-        <v>136</v>
-      </c>
-      <c r="E18" s="84" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="91" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="31">
-        <v>3</v>
-      </c>
-      <c r="J18" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K18" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L18" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="90" t="s">
-        <v>148</v>
-      </c>
-      <c r="N18" s="89" t="s">
-        <v>109</v>
-      </c>
-      <c r="O18" s="88" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="B19" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="85" t="s">
-        <v>131</v>
-      </c>
-      <c r="D19" s="85" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="84" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="31">
-        <v>3</v>
-      </c>
-      <c r="J19" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K19" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M19" s="89" t="s">
-        <v>149</v>
-      </c>
-      <c r="N19" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="O19" s="88" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="D20" s="85" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="85" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="91" t="s">
-        <v>146</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="31">
-        <v>3</v>
-      </c>
-      <c r="J20" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K20" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" s="89" t="s">
-        <v>150</v>
-      </c>
-      <c r="N20" s="89" t="s">
-        <v>122</v>
-      </c>
-      <c r="O20" s="88" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="85" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="85" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="85" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="91" t="s">
-        <v>147</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="31">
-        <v>3</v>
-      </c>
-      <c r="J21" s="32">
-        <v>44902</v>
-      </c>
-      <c r="K21" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L21" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="89" t="s">
-        <v>151</v>
-      </c>
-      <c r="N21" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="O21" s="88" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="7"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="8"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M29" s="5"/>
-    </row>
-    <row r="30" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M30" s="5"/>
+      <c r="O30" s="41" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="31" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I31" s="1"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="90"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="M31" s="5"/>
     </row>
     <row r="32" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I32" s="1"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="90"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="9:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I33" s="1"/>
+    <row r="33" spans="7:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="89"/>
+      <c r="H33" s="92"/>
+      <c r="I33" s="90"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="9:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I34" s="1"/>
+    </row>
+    <row r="34" spans="7:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="89"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="90"/>
       <c r="J34" s="1"/>
       <c r="K34" s="2"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I35" s="1"/>
+    <row r="35" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="90"/>
       <c r="J35" s="1"/>
       <c r="K35" s="2"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I36" s="1"/>
+    <row r="36" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="90"/>
       <c r="J36" s="1"/>
       <c r="K36" s="2"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I37" s="1"/>
+    <row r="37" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="90"/>
       <c r="J37" s="1"/>
       <c r="K37" s="2"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I38" s="1"/>
+    <row r="38" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="90"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="3"/>
-    </row>
-    <row r="39" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I39" s="1"/>
+      <c r="K38" s="94" t="s">
+        <v>2</v>
+      </c>
+      <c r="L38" s="95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="89"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="90"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="3"/>
-    </row>
-    <row r="40" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I40" s="1"/>
+      <c r="K39" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="L39" s="95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="89"/>
+      <c r="H40" s="92"/>
+      <c r="I40" s="90"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="3"/>
-    </row>
-    <row r="41" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I41" s="1"/>
+      <c r="K40" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="L40" s="95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="93"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="90"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="3"/>
-    </row>
-    <row r="42" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I42" s="1"/>
+      <c r="K41" s="94"/>
+      <c r="L41" s="95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="93"/>
+      <c r="H42" s="92"/>
+      <c r="I42" s="90"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="3"/>
-    </row>
-    <row r="43" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I43" s="1"/>
+      <c r="K42" s="94"/>
+      <c r="L42" s="96"/>
+    </row>
+    <row r="43" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="93"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="90"/>
       <c r="J43" s="1"/>
       <c r="K43" s="2"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I44" s="1"/>
+    <row r="44" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="93"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="90"/>
       <c r="J44" s="1"/>
       <c r="K44" s="2"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I45" s="1"/>
+    <row r="45" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="90"/>
       <c r="J45" s="1"/>
       <c r="K45" s="2"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I46" s="1"/>
+    <row r="46" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="90"/>
       <c r="J46" s="1"/>
       <c r="K46" s="2"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I47" s="1"/>
+    <row r="47" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
+      <c r="I47" s="90"/>
       <c r="J47" s="1"/>
       <c r="K47" s="2"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="2"/>
@@ -4427,11 +4954,11 @@
     <mergeCell ref="B3:O3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L6:L21" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$L$29:$L$32</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L6:L30" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$L$38:$L$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K6:K21" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$K$29:$K$31</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K6:K30" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>$K$38:$K$40</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -4464,415 +4991,415 @@
     <row r="2" spans="2:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="2:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="64"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="71"/>
     </row>
     <row r="7" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
     </row>
     <row r="8" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="16"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="13"/>
     </row>
     <row r="9" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="63" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="63" t="s">
+      <c r="F9" s="71"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="21"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="17"/>
-      <c r="C10" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="65" t="str">
+      <c r="B10" s="14"/>
+      <c r="C10" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="73" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,5,0)</f>
         <v>Administrator</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="65" t="str">
+      <c r="F10" s="71"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="73" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,11,0)</f>
         <v>Terminado</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="11" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="21"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="18"/>
     </row>
     <row r="12" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="63" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="63" t="s">
+      <c r="F12" s="71"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="64"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="21"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="18"/>
     </row>
     <row r="13" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="17"/>
-      <c r="C13" s="22">
+      <c r="B13" s="14"/>
+      <c r="C13" s="19">
         <f>VLOOKUP('User Stories'!C10,'Product Backlog- HU'!B6:O21,8,0)</f>
         <v>3</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="65" t="str">
+      <c r="D13" s="20"/>
+      <c r="E13" s="73" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="65" t="str">
+      <c r="F13" s="71"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="73" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,7,0)</f>
-        <v>Erick Maldonado</v>
-      </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="21"/>
+        <v>Mateo Loachamin</v>
+      </c>
+      <c r="I13" s="71"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="18"/>
     </row>
     <row r="14" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="17"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="18"/>
     </row>
     <row r="15" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="17"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="75" t="str">
+      <c r="D15" s="74" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,3,0)</f>
         <v>Add Prodcuts</v>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="45" t="s">
+      <c r="E15" s="54"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="75" t="str">
+      <c r="H15" s="74" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,4,0)</f>
         <v>Registration of products in inventory</v>
       </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="45" t="s">
+      <c r="I15" s="75"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="48" t="str">
+      <c r="M15" s="60" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,6,0)</f>
         <v>You enter the module to add products, click and enter the information of the products. The system calculates the business rules(subtotal, total_iva,unit:profit,total_profit)</v>
       </c>
-      <c r="N15" s="49"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="21"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="18"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="53"/>
-      <c r="P16" s="21"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="65"/>
+      <c r="P16" s="18"/>
     </row>
     <row r="17" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="17"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="21"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="18"/>
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="17"/>
-      <c r="C19" s="66" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="57" t="str">
+      <c r="D19" s="54"/>
+      <c r="E19" s="83" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,14,0)</f>
         <v>Add Products  to the system</v>
       </c>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="21"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="84"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="84"/>
+      <c r="N19" s="84"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="18"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="17"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="21"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="88"/>
+      <c r="P20" s="18"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="17"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="21"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="18"/>
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="17"/>
-      <c r="C22" s="70" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="48" t="str">
+      <c r="D22" s="54"/>
+      <c r="E22" s="60" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,12,0)</f>
         <v>The interface shows the screen to add products</v>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="70" t="s">
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="67"/>
-      <c r="L22" s="48" t="str">
+      <c r="K22" s="54"/>
+      <c r="L22" s="60" t="str">
         <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O21,13,0)</f>
         <v>It is necessary that the system allows to correctly add the data to the database</v>
       </c>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="21"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="18"/>
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="17"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="21"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="18"/>
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="17"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="21"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="18"/>
     </row>
     <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="26"/>
     </row>
     <row r="26" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5851,6 +6378,11 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D24"/>
@@ -5867,11 +6399,6 @@
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:J17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:O17"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>